<commit_message>
vault backup: 2021-10-29 16:46:35
Affected files:
.obsidian/workspace
1\351\231\204\344\273\266/MDM\346\235\203\351\231\220\347\256\241\347\220\206.xlsx
3\345\267\245\344\275\234\346\227\245\345\277\227/2021-10-29.md
</commit_message>
<xml_diff>
--- a/1附件/MDM权限管理.xlsx
+++ b/1附件/MDM权限管理.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35DE7EC-3DDE-7B4A-B7FB-6830B83F7325}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAD0018-E3C1-484B-9D36-8BF72D70EDC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-1600" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="298">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -725,14 +725,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>web登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单点登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>数据字典</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1198,6 +1190,18 @@
   </si>
   <si>
     <t>管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动应用授权</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web系统登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动应用登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2675,7 +2679,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2894,7 +2898,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>295</v>
       </c>
       <c r="B12" t="s">
         <v>172</v>
@@ -2925,7 +2929,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="B14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -2935,42 +2939,42 @@
       </c>
     </row>
     <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" t="s">
+        <v>294</v>
+      </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
         <v>150</v>
       </c>
-      <c r="E15" t="s">
-        <v>145</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="H16" t="s">
         <v>151</v>
       </c>
-      <c r="G15" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="B16" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>176</v>
-      </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>293</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2980,19 +2984,31 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="B18" t="s">
-        <v>179</v>
-      </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>110</v>
+      </c>
+      <c r="E18" t="s">
+        <v>265</v>
+      </c>
+      <c r="F18" t="s">
+        <v>266</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>150</v>
+      </c>
+      <c r="I18" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="B19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -3003,7 +3019,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="B20" t="s">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -3013,103 +3029,94 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" t="s">
-        <v>105</v>
-      </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" t="s">
+        <v>151</v>
+      </c>
+      <c r="G21" t="s">
+        <v>158</v>
+      </c>
+      <c r="H21" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>259</v>
+      </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22" t="s">
-        <v>182</v>
-      </c>
-      <c r="F22" t="s">
-        <v>294</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="B23" t="s">
-        <v>180</v>
-      </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:9">
+      <c r="B24" t="s">
+        <v>260</v>
+      </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>183</v>
-      </c>
-      <c r="E24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F24" t="s">
-        <v>185</v>
-      </c>
-      <c r="G24" t="s">
-        <v>164</v>
-      </c>
-      <c r="H24" t="s">
-        <v>186</v>
-      </c>
-      <c r="I24" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="B25" t="s">
-        <v>188</v>
-      </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:9">
+      <c r="B26" t="s">
+        <v>261</v>
+      </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" t="s">
-        <v>295</v>
+        <v>262</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -3119,26 +3126,17 @@
       </c>
     </row>
     <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" t="s">
+        <v>297</v>
+      </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" t="s">
-        <v>267</v>
-      </c>
-      <c r="F29" t="s">
-        <v>268</v>
-      </c>
-      <c r="G29" t="s">
-        <v>60</v>
-      </c>
-      <c r="H29" t="s">
-        <v>150</v>
-      </c>
-      <c r="I29" t="s">
-        <v>151</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3153,31 +3151,19 @@
       </c>
     </row>
     <row r="31" spans="1:9">
+      <c r="B31" t="s">
+        <v>177</v>
+      </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" t="s">
-        <v>268</v>
-      </c>
-      <c r="F31" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" t="s">
-        <v>150</v>
-      </c>
-      <c r="H31" t="s">
-        <v>151</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>260</v>
-      </c>
       <c r="B32" t="s">
-        <v>261</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -3186,75 +3172,99 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" t="s">
-        <v>262</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="C34" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
+        <v>179</v>
+      </c>
+      <c r="E34" t="s">
+        <v>180</v>
+      </c>
+      <c r="F34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="B35" t="s">
+        <v>178</v>
+      </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" t="s">
-        <v>263</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="C36" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
+        <v>181</v>
+      </c>
+      <c r="E36" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G36" t="s">
+        <v>164</v>
+      </c>
+      <c r="H36" t="s">
+        <v>184</v>
+      </c>
+      <c r="I36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="B37" t="s">
+        <v>186</v>
+      </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" t="s">
-        <v>264</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="C38" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
+        <v>187</v>
+      </c>
+      <c r="E38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3281,10 +3291,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3295,10 +3305,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3312,30 +3322,30 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" t="s">
         <v>192</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>193</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>194</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>195</v>
-      </c>
-      <c r="H3" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="D4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>
@@ -3343,10 +3353,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -3360,13 +3370,13 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F6" t="s">
         <v>232</v>
-      </c>
-      <c r="E6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F6" t="s">
-        <v>234</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -3377,10 +3387,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3394,10 +3404,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
@@ -3408,7 +3418,7 @@
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -3422,7 +3432,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="B10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -3436,7 +3446,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -3450,10 +3460,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -3467,13 +3477,13 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" t="s">
         <v>207</v>
-      </c>
-      <c r="E13" t="s">
-        <v>208</v>
-      </c>
-      <c r="F13" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3481,7 +3491,7 @@
         <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -3495,15 +3505,15 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -3514,7 +3524,7 @@
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -3528,21 +3538,21 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F18" t="s">
         <v>215</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>216</v>
-      </c>
-      <c r="F18" t="s">
-        <v>217</v>
-      </c>
-      <c r="G18" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -3562,10 +3572,10 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -3584,7 +3594,7 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3616,7 +3626,7 @@
         <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3627,7 +3637,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3638,7 +3648,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -3649,10 +3659,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -3663,10 +3673,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -3680,24 +3690,24 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" t="s">
         <v>240</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>241</v>
-      </c>
-      <c r="F6" t="s">
-        <v>242</v>
-      </c>
-      <c r="G6" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3714,13 +3724,13 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G8" t="s">
         <v>245</v>
-      </c>
-      <c r="F8" t="s">
-        <v>246</v>
-      </c>
-      <c r="G8" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3744,7 +3754,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -3758,18 +3768,18 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -3783,18 +3793,18 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E14" t="s">
+        <v>252</v>
+      </c>
+      <c r="F14" t="s">
         <v>253</v>
-      </c>
-      <c r="E14" t="s">
-        <v>254</v>
-      </c>
-      <c r="F14" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -3808,7 +3818,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3841,15 +3851,15 @@
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -3860,7 +3870,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -3874,13 +3884,13 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
+        <v>289</v>
+      </c>
+      <c r="E22" t="s">
         <v>291</v>
       </c>
-      <c r="E22" t="s">
-        <v>293</v>
-      </c>
       <c r="F22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3921,10 +3931,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3941,10 +3951,10 @@
         <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G3" t="s">
         <v>60</v>
@@ -3952,7 +3962,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -3969,10 +3979,10 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G5" t="s">
         <v>60</v>
@@ -3980,7 +3990,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -3997,10 +4007,10 @@
         <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G7" t="s">
         <v>60</v>
@@ -4008,7 +4018,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -4027,10 +4037,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -4049,10 +4059,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -4077,10 +4087,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -4094,7 +4104,7 @@
         <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -4111,10 +4121,10 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G16" t="s">
         <v>60</v>
@@ -4122,7 +4132,7 @@
     </row>
     <row r="17" spans="2:5">
       <c r="B17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -4136,7 +4146,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -4155,12 +4165,12 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -4190,7 +4200,7 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -4215,15 +4225,15 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -4237,15 +4247,15 @@
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -4259,15 +4269,15 @@
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -4289,7 +4299,7 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -4311,7 +4321,7 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -4353,10 +4363,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -4370,12 +4380,12 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -4389,12 +4399,12 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -4408,12 +4418,12 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -4427,12 +4437,12 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -4446,12 +4456,12 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -4465,7 +4475,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4473,7 +4483,7 @@
         <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>

</xml_diff>